<commit_message>
Changes in column name
</commit_message>
<xml_diff>
--- a/Promos Fotos Datos.xlsx
+++ b/Promos Fotos Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darwin\Documents\proyecto mil\checho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4461C73A-9F09-423B-A76B-8CB400DBB77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA34F74-62F9-4089-B857-8042D41EDA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -638,9 +638,6 @@
     <t>https://assets.adidas.com/images/h_840,f_auto,q_auto,fl_lossy,c_fill,g_auto/6c08c5915c0f4c6eb5ab109dd6616f0a_9366/5_PANEL_TRUCKER_Multicolor_IQ2895_01_standard.jpg</t>
   </si>
   <si>
-    <t>Texto Personalizado</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -651,6 +648,9 @@
   </si>
   <si>
     <t>https://lh3.googleusercontent.com/pw/AP1GczOTvbCZTs5jYE772Pg0CQiFlFBlIAeBUnk776t0W8uEQNNj25L1zXPJJAio7e3RiD7EdpCcdVAtIJFCMz0kZXNWytv01Nm9loX1XlGo-E81_NYdmnZ6eZHUpU-34wBh1Nj_UEAvh6PDUIjzzKw3q_Kj=w467-h460-s-no-gm?authuser=5</t>
+  </si>
+  <si>
+    <t>Full image</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -693,6 +693,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -728,7 +735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -753,6 +760,7 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -998,8 +1006,8 @@
   <dimension ref="A1:T205"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1049,8 +1057,8 @@
       <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>205</v>
+      <c r="K1" s="12" t="s">
+        <v>209</v>
       </c>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
@@ -1155,7 +1163,7 @@
         <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
@@ -1227,7 +1235,7 @@
         <v>29</v>
       </c>
       <c r="K6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
@@ -1326,7 +1334,7 @@
         <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
@@ -1392,7 +1400,7 @@
         <v>25</v>
       </c>
       <c r="K11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1">
@@ -1473,7 +1481,7 @@
         <v>54</v>
       </c>
       <c r="K14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="15.75" customHeight="1">
@@ -1523,7 +1531,7 @@
         <v>16</v>
       </c>
       <c r="K16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
@@ -1601,7 +1609,7 @@
         <v>25</v>
       </c>
       <c r="K19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
@@ -1661,7 +1669,7 @@
         <v>76</v>
       </c>
       <c r="K21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
@@ -1738,7 +1746,7 @@
         <v>25</v>
       </c>
       <c r="K24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
@@ -1791,7 +1799,7 @@
         <v>91</v>
       </c>
       <c r="K26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
@@ -1869,7 +1877,7 @@
         <v>25</v>
       </c>
       <c r="K29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
@@ -1922,7 +1930,7 @@
         <v>25</v>
       </c>
       <c r="K31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1">
@@ -1997,7 +2005,7 @@
         <v>5</v>
       </c>
       <c r="K34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
@@ -2054,7 +2062,7 @@
         <v>14</v>
       </c>
       <c r="K36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
@@ -2138,7 +2146,7 @@
         <v>25</v>
       </c>
       <c r="K39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1">
@@ -2192,7 +2200,7 @@
         <v>25</v>
       </c>
       <c r="K41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1">
@@ -2276,7 +2284,7 @@
         <v>25</v>
       </c>
       <c r="K44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1">
@@ -2328,7 +2336,7 @@
         <v>25</v>
       </c>
       <c r="K46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1">
@@ -2409,7 +2417,7 @@
         <v>15</v>
       </c>
       <c r="K49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1">
@@ -2463,7 +2471,7 @@
         <v>15</v>
       </c>
       <c r="K51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="15.75" customHeight="1">
@@ -2544,7 +2552,7 @@
         <v>25</v>
       </c>
       <c r="K54" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="15.75" customHeight="1">
@@ -2598,7 +2606,7 @@
         <v>25</v>
       </c>
       <c r="K56" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="15.75" customHeight="1">
@@ -2682,7 +2690,7 @@
         <v>14</v>
       </c>
       <c r="K59" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="15.75" customHeight="1">
@@ -2703,7 +2711,7 @@
         <v>256334</v>
       </c>
       <c r="G60" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H60">
         <v>26</v>
@@ -2733,7 +2741,7 @@
         <v>256335</v>
       </c>
       <c r="G61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H61">
         <v>27</v>
@@ -2763,7 +2771,7 @@
         <v>256336</v>
       </c>
       <c r="G62" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H62">
         <v>28</v>

</xml_diff>